<commit_message>
Add additional tests and lintly fixes
</commit_message>
<xml_diff>
--- a/test_data/operations/electrical_requirements.xlsx
+++ b/test_data/operations/electrical_requirements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="110" windowWidth="22980" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="110" windowWidth="22980" windowHeight="8940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="On-Site" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>False</t>
   </si>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -882,15 +882,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
     <col min="2" max="2" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
@@ -907,7 +907,7 @@
     <col min="17" max="17" width="32.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -959,6 +959,231 @@
       <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="2" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>6</v>
+      </c>
+      <c r="L3" s="1">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>6</v>
+      </c>
+      <c r="P3" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>6</v>
+      </c>
+      <c r="L4" s="1">
+        <v>15</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>6</v>
+      </c>
+      <c r="P4" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>48</v>
+      </c>
+      <c r="F5" s="1">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>6</v>
+      </c>
+      <c r="L5" s="1">
+        <v>15</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>6</v>
+      </c>
+      <c r="P5" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>